<commit_message>
Save changes to AUTO.xlsx
</commit_message>
<xml_diff>
--- a/AUTO.xlsx
+++ b/AUTO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\holdem-auto-trader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corea\Desktop\holdem-auto-trader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5687698-08F1-4134-83BA-05973F55487C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2B6880-DBC3-49B2-B6A7-F0BBAD7776E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{AB34D403-B5C5-434B-8E46-EDEFA1840EDF}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{AB34D403-B5C5-434B-8E46-EDEFA1840EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="12">
   <si>
     <t>P</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,12 +130,6 @@
   <si>
     <t>N</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
 </sst>
 </file>
@@ -1297,39 +1291,17 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1393,18 +1365,18 @@
       <c r="BU3" s="2"/>
       <c r="BV3" s="2"/>
       <c r="BW3" s="7"/>
-      <c r="BX3" s="11">
+      <c r="BX3" s="11" t="str">
         <f>IF(B3="","",COUNTIF(B3:BW3,"P"))</f>
-        <v>4</v>
-      </c>
-      <c r="BY3" s="12">
+        <v/>
+      </c>
+      <c r="BY3" s="12" t="str">
         <f>IF(B3="","",COUNTIF(B3:BW3,"B"))</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="BZ3" s="12"/>
-      <c r="CA3" s="13">
+      <c r="CA3" s="13" t="str">
         <f>IF(B3="","",BX3+BY3)</f>
-        <v>11</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:79" ht="17.25" thickBot="1">
@@ -2242,47 +2214,47 @@
       </c>
       <c r="C12" s="2" t="str">
         <f>IF(AI!C11="","",AI!C11)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D12" s="2" t="str">
         <f>IF(AI!D11="","",AI!D11)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E12" s="2" t="str">
         <f>IF(AI!E11="","",AI!E11)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F12" s="2" t="str">
         <f>IF(AI!F11="","",AI!F11)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G12" s="2" t="str">
         <f>IF(AI!G11="","",AI!G11)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H12" s="2" t="str">
         <f>IF(AI!H11="","",AI!H11)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="I12" s="2" t="str">
         <f>IF(AI!I11="","",AI!I11)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="J12" s="2" t="str">
         <f>IF(AI!J11="","",AI!J11)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="K12" s="2" t="str">
         <f>IF(AI!K11="","",AI!K11)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="L12" s="2" t="str">
         <f>IF(AI!L11="","",AI!L11)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="M12" s="2" t="str">
         <f>IF(AI!M11="","",AI!M11)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="N12" s="2" t="str">
         <f>IF(AI!N11="","",AI!N11)</f>
@@ -2861,47 +2833,47 @@
       </c>
       <c r="B16" s="2" t="str">
         <f>IF(AI!B12="","",AI!B12)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="C16" s="2" t="str">
         <f>IF(AI!C12="","",AI!C12)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D16" s="2" t="str">
         <f>IF(AI!D12="","",AI!D12)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E16" s="2" t="str">
         <f>IF(AI!E12="","",AI!E12)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F16" s="2" t="str">
         <f>IF(AI!F12="","",AI!F12)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G16" s="2" t="str">
         <f>IF(AI!G12="","",AI!G12)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H16" s="2" t="str">
         <f>IF(AI!H12="","",AI!H12)</f>
-        <v>L</v>
+        <v/>
       </c>
       <c r="I16" s="2" t="str">
         <f>IF(AI!I12="","",AI!I12)</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="J16" s="2" t="str">
         <f>IF(AI!J12="","",AI!J12)</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="K16" s="2" t="str">
         <f>IF(AI!K12="","",AI!K12)</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="L16" s="2" t="str">
         <f>IF(AI!L12="","",AI!L12)</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="M16" s="2" t="str">
         <f>IF(AI!M12="","",AI!M12)</f>
@@ -3155,18 +3127,18 @@
         <f>IF(AI!BW12="","",AI!BW12)</f>
         <v/>
       </c>
-      <c r="BX16" s="11">
+      <c r="BX16" s="11" t="str">
         <f>IF(B16="","",COUNTIF(B16:BW16,"W"))</f>
-        <v>4</v>
-      </c>
-      <c r="BY16" s="12">
+        <v/>
+      </c>
+      <c r="BY16" s="12" t="str">
         <f>IF(B16="","",COUNTIF(B16:BW16,"L"))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="BZ16" s="12"/>
-      <c r="CA16" s="13">
+      <c r="CA16" s="13" t="str">
         <f>IF(B16="","",BX16-BY16)</f>
-        <v>3</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:79" ht="17.25" thickBot="1">
@@ -4359,47 +4331,47 @@
       </c>
       <c r="B2" s="15" t="str">
         <f>IF(DATA!B3="","",DATA!B3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="C2" s="15" t="str">
         <f>IF(DATA!C3="","",DATA!C3)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="D2" s="15" t="str">
         <f>IF(DATA!D3="","",DATA!D3)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="E2" s="15" t="str">
         <f>IF(DATA!E3="","",DATA!E3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="F2" s="15" t="str">
         <f>IF(DATA!F3="","",DATA!F3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="G2" s="15" t="str">
         <f>IF(DATA!G3="","",DATA!G3)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="H2" s="15" t="str">
         <f>IF(DATA!H3="","",DATA!H3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="I2" s="15" t="str">
         <f>IF(DATA!I3="","",DATA!I3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="J2" s="15" t="str">
         <f>IF(DATA!J3="","",DATA!J3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="K2" s="15" t="str">
         <f>IF(DATA!K3="","",DATA!K3)</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="L2" s="15" t="str">
         <f>IF(DATA!L3="","",DATA!L3)</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="M2" s="15" t="str">
         <f>IF(DATA!M3="","",DATA!M3)</f>
@@ -4647,51 +4619,51 @@
       </c>
       <c r="C3" s="15" t="str">
         <f>IF(B2="","","N")</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D3" s="15" t="str">
         <f>IF(C2="","","N")</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E3" s="15" t="str">
         <f>IF(D2="","","N")</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F3" s="15" t="str">
         <f>IF(E2="","",
 IF(AND(B2&lt;&gt;C2,C2=D2),IF(B2=C2,E2,IF(B2&lt;&gt;C2,IF(E2="P","B","P"))),
 IF(B2=C2,E2,IF(E2="P","B","P"))))</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="G3" s="15" t="str">
         <f t="shared" ref="G3:BR3" si="0">IF(F2="","",
 IF(AND(C2&lt;&gt;D2,D2=E2),IF(C2=D2,F2,IF(C2&lt;&gt;D2,IF(F2="P","B","P"))),
 IF(C2=D2,F2,IF(F2="P","B","P"))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="H3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="I3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="J3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="K3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="L3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="M3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="N3" s="15" t="str">
         <f t="shared" si="0"/>
@@ -4936,49 +4908,49 @@
         <f>IF(B$2="","",
 IF(B3="N","N",
 IF(B$2=B3,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="C4" s="15" t="str">
         <f t="shared" ref="C4:BN4" si="2">IF(C$2="","",
 IF(C3="N","N",
 IF(C$2=C3,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="G4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="H4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>W</v>
+        <v/>
       </c>
       <c r="I4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>W</v>
+        <v/>
       </c>
       <c r="J4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="K4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="L4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="M4" s="15" t="str">
         <f t="shared" si="2"/>
@@ -5229,56 +5201,56 @@
       </c>
       <c r="C5" s="15" t="str">
         <f t="shared" ref="C5:G5" si="4">IF(C3="","","N")</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D5" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E5" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F5" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G5" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H5" s="17" t="str">
         <f t="shared" ref="H5:K5" si="5">IF(H3="","",
 IF(H3="N","N",
 IF(COUNTIF(D4:G4,"W")&gt;=2,H3,
 IF(COUNTIF(D4:G4,"W")&lt;2,IF(H3="P","B","P")))))</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="I5" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="J5" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="K5" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="L5" s="17" t="str">
         <f>IF(L3="","",
 IF(L3="N","N",
 IF(COUNTIF(H4:K4,"W")&gt;=2,L3,
 IF(COUNTIF(H4:K4,"W")&lt;2,IF(L3="P","B","P")))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="M5" s="17" t="str">
         <f t="shared" ref="M5:BS5" si="6">IF(M3="","",
 IF(M3="N","N",
 IF(COUNTIF(I4:L4,"W")&gt;=2,M3,
 IF(COUNTIF(I4:L4,"W")&lt;2,IF(M3="P","B","P")))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="N5" s="17" t="str">
         <f t="shared" si="6"/>
@@ -5521,49 +5493,49 @@
         <f>IF(B$2="","",
 IF(B5="N","N",
 IF(B$2=B5,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="C6" s="15" t="str">
         <f t="shared" ref="C6:BN6" si="7">IF(C$2="","",
 IF(C5="N","N",
 IF(C$2=C5,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="I6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="J6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="K6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="L6" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>L</v>
+        <v/>
       </c>
       <c r="M6" s="15" t="str">
         <f t="shared" si="7"/>
@@ -5816,53 +5788,53 @@
       </c>
       <c r="C7" s="15" t="str">
         <f t="shared" ref="C7:H7" si="10">IF(C5="","",C5)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D7" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E7" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F7" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G7" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H7" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="I7" s="17" t="str">
         <f>IF(I5="","",
 IF(I5="N","N",
 IF(H6="W",I5,
 IF(H6="L",IF(I5="P","B","P")))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="J7" s="17" t="str">
         <f t="shared" ref="J7:BS7" si="11">IF(J5="","",
 IF(J5="N","N",
 IF(I6="W",J5,
 IF(I6="L",IF(J5="P","B","P")))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="K7" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="L7" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="M7" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="N7" s="17" t="str">
         <f t="shared" si="11"/>
@@ -6105,67 +6077,67 @@
         <f>IF(B$2="","",
 IF(B7="N","N",
 IF(B$2=B7,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="C8" s="15" t="str">
         <f t="shared" ref="C8" si="12">IF(C$2="","",
 IF(C7="N","N",
 IF(C$2=C7,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D8" s="15" t="str">
         <f t="shared" ref="D8" si="13">IF(D$2="","",
 IF(D7="N","N",
 IF(D$2=D7,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E8" s="15" t="str">
         <f t="shared" ref="E8" si="14">IF(E$2="","",
 IF(E7="N","N",
 IF(E$2=E7,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F8" s="15" t="str">
         <f t="shared" ref="F8" si="15">IF(F$2="","",
 IF(F7="N","N",
 IF(F$2=F7,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G8" s="15" t="str">
         <f t="shared" ref="G8" si="16">IF(G$2="","",
 IF(G7="N","N",
 IF(G$2=G7,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H8" s="15" t="str">
         <f t="shared" ref="H8" si="17">IF(H$2="","",
 IF(H7="N","N",
 IF(H$2=H7,"W","L")))</f>
-        <v>L</v>
+        <v/>
       </c>
       <c r="I8" s="15" t="str">
         <f t="shared" ref="I8" si="18">IF(I$2="","",
 IF(I7="N","N",
 IF(I$2=I7,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="J8" s="15" t="str">
         <f t="shared" ref="J8" si="19">IF(J$2="","",
 IF(J7="N","N",
 IF(J$2=J7,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="K8" s="15" t="str">
         <f t="shared" ref="K8" si="20">IF(K$2="","",
 IF(K7="N","N",
 IF(K$2=K7,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="L8" s="15" t="str">
         <f t="shared" ref="L8" si="21">IF(L$2="","",
 IF(L7="N","N",
 IF(L$2=L7,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="M8" s="15" t="str">
         <f t="shared" ref="M8" si="22">IF(M$2="","",
@@ -6532,50 +6504,50 @@
       </c>
       <c r="C9" s="15" t="str">
         <f t="shared" ref="C9:I9" si="81">IF(C7="","",C7)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="I9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="J9" s="17" t="str">
         <f t="shared" ref="J9:BS9" si="82">IF(J7="","",
 IF(J7="N","N",
 IF(I8="W",J7,
 IF(I8="L",IF(J7="P","B","P")))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="K9" s="17" t="str">
         <f t="shared" si="82"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="L9" s="17" t="str">
         <f t="shared" si="82"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="M9" s="17" t="str">
         <f t="shared" si="82"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="N9" s="17" t="str">
         <f t="shared" si="82"/>
@@ -6818,67 +6790,67 @@
         <f>IF(B$2="","",
 IF(B9="N","N",
 IF(B$2=B9,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="C10" s="15" t="str">
         <f t="shared" ref="C10" si="83">IF(C$2="","",
 IF(C9="N","N",
 IF(C$2=C9,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D10" s="15" t="str">
         <f t="shared" ref="D10" si="84">IF(D$2="","",
 IF(D9="N","N",
 IF(D$2=D9,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E10" s="15" t="str">
         <f t="shared" ref="E10" si="85">IF(E$2="","",
 IF(E9="N","N",
 IF(E$2=E9,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F10" s="15" t="str">
         <f t="shared" ref="F10" si="86">IF(F$2="","",
 IF(F9="N","N",
 IF(F$2=F9,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G10" s="15" t="str">
         <f t="shared" ref="G10" si="87">IF(G$2="","",
 IF(G9="N","N",
 IF(G$2=G9,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H10" s="15" t="str">
         <f t="shared" ref="H10" si="88">IF(H$2="","",
 IF(H9="N","N",
 IF(H$2=H9,"W","L")))</f>
-        <v>L</v>
+        <v/>
       </c>
       <c r="I10" s="15" t="str">
         <f t="shared" ref="I10" si="89">IF(I$2="","",
 IF(I9="N","N",
 IF(I$2=I9,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="J10" s="15" t="str">
         <f t="shared" ref="J10" si="90">IF(J$2="","",
 IF(J9="N","N",
 IF(J$2=J9,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="K10" s="15" t="str">
         <f t="shared" ref="K10" si="91">IF(K$2="","",
 IF(K9="N","N",
 IF(K$2=K9,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="L10" s="15" t="str">
         <f t="shared" ref="L10" si="92">IF(L$2="","",
 IF(L9="N","N",
 IF(L$2=L9,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="M10" s="15" t="str">
         <f t="shared" ref="M10" si="93">IF(M$2="","",
@@ -7245,56 +7217,56 @@
       </c>
       <c r="C11" s="15" t="str">
         <f t="shared" ref="C11:J11" si="152">IF(C9="","",C9)</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>P</v>
+        <v/>
       </c>
       <c r="I11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="J11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>B</v>
+        <v/>
       </c>
       <c r="K11" s="17" t="str">
         <f t="shared" ref="K11" si="153">IF(K9="","",
 IF(K9="N","N",
 IF(COUNTIF(G10:J10,"W")&gt;=2,K9,
 IF(COUNTIF(G10:J10,"W")&lt;2,IF(K9="P","B","P")))))</f>
-        <v>B</v>
+        <v/>
       </c>
       <c r="L11" s="17" t="str">
         <f t="shared" ref="L11" si="154">IF(L9="","",
 IF(L9="N","N",
 IF(COUNTIF(H10:K10,"W")&gt;=2,L9,
 IF(COUNTIF(H10:K10,"W")&lt;2,IF(L9="P","B","P")))))</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="M11" s="17" t="str">
         <f t="shared" ref="M11" si="155">IF(M9="","",
 IF(M9="N","N",
 IF(COUNTIF(I10:L10,"W")&gt;=2,M9,
 IF(COUNTIF(I10:L10,"W")&lt;2,IF(M9="P","B","P")))))</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="N11" s="17" t="str">
         <f t="shared" ref="N11" si="156">IF(N9="","",
@@ -7711,67 +7683,67 @@
         <f>IF(B$2="","",
 IF(B11="N","N",
 IF(B$2=B11,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="C12" s="15" t="str">
         <f t="shared" ref="C12" si="214">IF(C$2="","",
 IF(C11="N","N",
 IF(C$2=C11,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="D12" s="15" t="str">
         <f t="shared" ref="D12" si="215">IF(D$2="","",
 IF(D11="N","N",
 IF(D$2=D11,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="E12" s="15" t="str">
         <f t="shared" ref="E12" si="216">IF(E$2="","",
 IF(E11="N","N",
 IF(E$2=E11,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="F12" s="15" t="str">
         <f t="shared" ref="F12" si="217">IF(F$2="","",
 IF(F11="N","N",
 IF(F$2=F11,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="G12" s="15" t="str">
         <f t="shared" ref="G12" si="218">IF(G$2="","",
 IF(G11="N","N",
 IF(G$2=G11,"W","L")))</f>
-        <v>N</v>
+        <v/>
       </c>
       <c r="H12" s="15" t="str">
         <f t="shared" ref="H12" si="219">IF(H$2="","",
 IF(H11="N","N",
 IF(H$2=H11,"W","L")))</f>
-        <v>L</v>
+        <v/>
       </c>
       <c r="I12" s="15" t="str">
         <f t="shared" ref="I12" si="220">IF(I$2="","",
 IF(I11="N","N",
 IF(I$2=I11,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="J12" s="15" t="str">
         <f t="shared" ref="J12" si="221">IF(J$2="","",
 IF(J11="N","N",
 IF(J$2=J11,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="K12" s="15" t="str">
         <f t="shared" ref="K12" si="222">IF(K$2="","",
 IF(K11="N","N",
 IF(K$2=K11,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="L12" s="15" t="str">
         <f t="shared" ref="L12" si="223">IF(L$2="","",
 IF(L11="N","N",
 IF(L$2=L11,"W","L")))</f>
-        <v>W</v>
+        <v/>
       </c>
       <c r="M12" s="15" t="str">
         <f t="shared" ref="M12" si="224">IF(M$2="","",

</xml_diff>

<commit_message>
room_entry_service.py 방 새로고침 타이밍 변경
</commit_message>
<xml_diff>
--- a/AUTO.xlsx
+++ b/AUTO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corea\Desktop\holdem-auto-trader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\holdem-auto-trader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48432498-C516-4FFC-988D-5B63B15FD9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F834385E-F038-4147-852D-2086F6C83610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{AB34D403-B5C5-434B-8E46-EDEFA1840EDF}"/>
+    <workbookView xWindow="7200" yWindow="3990" windowWidth="21600" windowHeight="11385" xr2:uid="{AB34D403-B5C5-434B-8E46-EDEFA1840EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -1298,10 +1298,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -1310,13 +1310,13 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
@@ -1325,7 +1325,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1393,11 +1393,11 @@
       <c r="BW3" s="7"/>
       <c r="BX3" s="11">
         <f>IF(B3="","",COUNTIF(B3:BW3,"P"))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BY3" s="12">
         <f>IF(B3="","",COUNTIF(B3:BW3,"B"))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BZ3" s="12"/>
       <c r="CA3" s="13">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="H12" s="2" t="str">
         <f>IF(AI!H11="","",AI!H11)</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="I12" s="2" t="str">
         <f>IF(AI!I11="","",AI!I11)</f>
@@ -2272,11 +2272,11 @@
       </c>
       <c r="K12" s="2" t="str">
         <f>IF(AI!K11="","",AI!K11)</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="L12" s="2" t="str">
         <f>IF(AI!L11="","",AI!L11)</f>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="M12" s="2" t="str">
         <f>IF(AI!M11="","",AI!M11)</f>
@@ -4357,11 +4357,11 @@
       </c>
       <c r="B2" s="15" t="str">
         <f>IF(DATA!B3="","",DATA!B3)</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>IF(DATA!C3="","",DATA!C3)</f>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="D2" s="15" t="str">
         <f>IF(DATA!D3="","",DATA!D3)</f>
@@ -4373,15 +4373,15 @@
       </c>
       <c r="F2" s="15" t="str">
         <f>IF(DATA!F3="","",DATA!F3)</f>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="G2" s="15" t="str">
         <f>IF(DATA!G3="","",DATA!G3)</f>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="H2" s="15" t="str">
         <f>IF(DATA!H3="","",DATA!H3)</f>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="I2" s="15" t="str">
         <f>IF(DATA!I3="","",DATA!I3)</f>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="K2" s="15" t="str">
         <f>IF(DATA!K3="","",DATA!K3)</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="L2" s="15" t="str">
         <f>IF(DATA!L3="","",DATA!L3)</f>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="H3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="I3" s="15" t="str">
         <f t="shared" si="0"/>
@@ -4952,11 +4952,11 @@
       </c>
       <c r="F4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v>W</v>
       </c>
       <c r="G4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>W</v>
+        <v>L</v>
       </c>
       <c r="H4" s="15" t="str">
         <f t="shared" si="2"/>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="K4" s="15" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v>W</v>
       </c>
       <c r="L4" s="15" t="str">
         <f t="shared" si="2"/>
@@ -5250,7 +5250,7 @@
 IF(H3="N","N",
 IF(COUNTIF(D4:G4,"W")&gt;=2,H3,
 IF(COUNTIF(D4:G4,"W")&lt;2,IF(H3="P","B","P")))))</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="I5" s="17" t="str">
         <f t="shared" si="5"/>
@@ -5262,14 +5262,14 @@
       </c>
       <c r="K5" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="L5" s="17" t="str">
         <f>IF(L3="","",
 IF(L3="N","N",
 IF(COUNTIF(H4:K4,"W")&gt;=2,L3,
 IF(COUNTIF(H4:K4,"W")&lt;2,IF(L3="P","B","P")))))</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="M5" s="17" t="str">
         <f t="shared" ref="M5:BS5" si="6">IF(M3="","",
@@ -5834,7 +5834,7 @@
       </c>
       <c r="H7" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="I7" s="17" t="str">
         <f>IF(I5="","",
@@ -5852,11 +5852,11 @@
       </c>
       <c r="K7" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="L7" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="M7" s="17" t="str">
         <f t="shared" si="11"/>
@@ -6550,7 +6550,7 @@
       </c>
       <c r="H9" s="15" t="str">
         <f t="shared" si="81"/>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="I9" s="15" t="str">
         <f t="shared" si="81"/>
@@ -6565,11 +6565,11 @@
       </c>
       <c r="K9" s="17" t="str">
         <f t="shared" si="82"/>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="L9" s="17" t="str">
         <f t="shared" si="82"/>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="M9" s="17" t="str">
         <f t="shared" si="82"/>
@@ -7263,7 +7263,7 @@
       </c>
       <c r="H11" s="15" t="str">
         <f t="shared" si="152"/>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="I11" s="15" t="str">
         <f t="shared" si="152"/>
@@ -7278,14 +7278,14 @@
 IF(K9="N","N",
 IF(COUNTIF(G10:J10,"W")&gt;=2,K9,
 IF(COUNTIF(G10:J10,"W")&lt;2,IF(K9="P","B","P")))))</f>
-        <v>B</v>
+        <v>P</v>
       </c>
       <c r="L11" s="17" t="str">
         <f t="shared" ref="L11" si="154">IF(L9="","",
 IF(L9="N","N",
 IF(COUNTIF(H10:K10,"W")&gt;=2,L9,
 IF(COUNTIF(H10:K10,"W")&lt;2,IF(L9="P","B","P")))))</f>
-        <v>P</v>
+        <v>B</v>
       </c>
       <c r="M11" s="17" t="str">
         <f t="shared" ref="M11" si="155">IF(M9="","",

</xml_diff>